<commit_message>
script structunig and inheritance
</commit_message>
<xml_diff>
--- a/PROJECT_TRACKER.xlsx
+++ b/PROJECT_TRACKER.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="620" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="620"/>
   </bookViews>
   <sheets>
     <sheet name="STATUS" sheetId="1" r:id="rId1"/>
@@ -495,6 +495,57 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,57 +566,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,31 +914,31 @@
       <c r="F2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
@@ -948,13 +948,13 @@
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="53"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -968,13 +968,13 @@
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="33"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -988,13 +988,13 @@
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="50"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
@@ -1004,13 +1004,13 @@
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="53"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
@@ -1022,15 +1022,15 @@
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="50"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="55"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -1042,13 +1042,13 @@
       </c>
       <c r="E9" s="26"/>
       <c r="F9" s="28"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="50"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="55"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -1060,13 +1060,13 @@
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="30"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="50"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="55"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
@@ -1076,13 +1076,13 @@
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="28"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="50"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="55"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -1094,13 +1094,13 @@
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="28"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="50"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="55"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
@@ -1110,13 +1110,13 @@
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="53"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
@@ -1126,13 +1126,13 @@
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="28"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="50"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="55"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
@@ -1142,13 +1142,13 @@
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="53"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
@@ -1158,13 +1158,13 @@
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="28"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="50"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="55"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
@@ -1174,13 +1174,13 @@
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="28"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="55"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
@@ -1190,13 +1190,13 @@
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="53"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
@@ -1206,13 +1206,13 @@
       </c>
       <c r="E19" s="31"/>
       <c r="F19" s="28"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="50"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="55"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
@@ -1222,13 +1222,13 @@
       </c>
       <c r="E20" s="31"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="50"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="55"/>
     </row>
     <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
@@ -1236,13 +1236,13 @@
       <c r="D21" s="39"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="43"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="60"/>
     </row>
     <row r="22" spans="2:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
@@ -1259,20 +1259,20 @@
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G23" s="46" t="s">
+      <c r="G23" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="46" t="s">
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="47"/>
-      <c r="M23" s="48"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="65"/>
     </row>
     <row r="24" spans="2:13" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="61" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="17"/>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="25" spans="2:13" s="1" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="37"/>
-      <c r="F25" s="45"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="21" t="s">
         <v>34</v>
       </c>
@@ -1310,6 +1310,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="G21:M21"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="G16:M16"/>
+    <mergeCell ref="G17:M17"/>
+    <mergeCell ref="G18:M18"/>
+    <mergeCell ref="G20:M20"/>
+    <mergeCell ref="G11:M11"/>
+    <mergeCell ref="G19:M19"/>
+    <mergeCell ref="G10:M10"/>
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="G13:M13"/>
+    <mergeCell ref="G14:M14"/>
+    <mergeCell ref="G15:M15"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="G7:M7"/>
@@ -1318,21 +1333,6 @@
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="G5:M5"/>
     <mergeCell ref="G6:M6"/>
-    <mergeCell ref="G11:M11"/>
-    <mergeCell ref="G19:M19"/>
-    <mergeCell ref="G10:M10"/>
-    <mergeCell ref="G12:M12"/>
-    <mergeCell ref="G13:M13"/>
-    <mergeCell ref="G14:M14"/>
-    <mergeCell ref="G15:M15"/>
-    <mergeCell ref="G21:M21"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="G16:M16"/>
-    <mergeCell ref="G17:M17"/>
-    <mergeCell ref="G18:M18"/>
-    <mergeCell ref="G20:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1343,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1368,7 @@
       <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="42" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="35" t="s">
@@ -1377,40 +1377,40 @@
       <c r="E3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="54"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="51"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
-    </row>
-    <row r="5" spans="2:12" s="65" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="58"/>
+    </row>
+    <row r="5" spans="2:12" s="49" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="64"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="66" t="s">
         <v>40</v>
       </c>
@@ -1424,158 +1424,158 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="38"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="38"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="50"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="38"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="50"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="55"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="38"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="50"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="55"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="38"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="50"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="55"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="38"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="50"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="55"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="38"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="55"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="38"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="50"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="55"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="38"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="50"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="55"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="38"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="50"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="55"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="38"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="50"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="55"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
       <c r="C17" s="39"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="43"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="60"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="16"/>
@@ -1592,21 +1592,21 @@
     </row>
     <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37"/>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="46" t="s">
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="47"/>
-      <c r="L19" s="48"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="65"/>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37"/>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="61" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="17"/>
@@ -1621,7 +1621,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="37"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="45"/>
+      <c r="E21" s="62"/>
       <c r="F21" s="21" t="s">
         <v>34</v>
       </c>
@@ -1649,11 +1649,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F16:L16"/>
-    <mergeCell ref="F17:L17"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="F5:L5"/>
+    <mergeCell ref="F6:L6"/>
     <mergeCell ref="F12:L12"/>
     <mergeCell ref="F13:L13"/>
     <mergeCell ref="F14:L14"/>
@@ -1663,10 +1662,11 @@
     <mergeCell ref="F9:L9"/>
     <mergeCell ref="F10:L10"/>
     <mergeCell ref="F11:L11"/>
-    <mergeCell ref="F3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="F5:L5"/>
-    <mergeCell ref="F6:L6"/>
+    <mergeCell ref="F16:L16"/>
+    <mergeCell ref="F17:L17"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>